<commit_message>
BIS-1002: Improvements to internal namespace tests in import
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/systemtest/asapi/v3/test_files/import/import_internal_type.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/systemtest/asapi/v3/test_files/import/import_internal_type.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TYPES" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="92">
   <si>
     <t xml:space="preserve">DATASET_TYPE</t>
   </si>
@@ -101,6 +101,9 @@
     <t xml:space="preserve">IST</t>
   </si>
   <si>
+    <t xml:space="preserve">Internal Assignment</t>
+  </si>
+  <si>
     <t xml:space="preserve">SUPPLIER</t>
   </si>
   <si>
@@ -171,6 +174,42 @@
   </si>
   <si>
     <t xml:space="preserve">Enter the code of the object type for which the collection is used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$FOR_WHAT_INTERNAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For what internal?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VOCABULARY_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$INTERNAL_VOCABULARY_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal Vocabulary Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$INTERNAL_TERM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">internal term for test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGULAR_TERM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regular term for test</t>
   </si>
   <si>
     <t xml:space="preserve">SPACE</t>
@@ -270,7 +309,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -299,13 +338,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -331,17 +364,37 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -355,14 +408,6 @@
       <b val="true"/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -417,7 +462,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -434,11 +479,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -446,23 +491,31 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -478,15 +531,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -494,15 +555,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -529,11 +590,11 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.3984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.83"/>
@@ -678,7 +739,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="19.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>1</v>
       </c>
@@ -709,8 +770,11 @@
       <c r="J10" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K10" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -735,10 +799,13 @@
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="5"/>
+      <c r="K11" s="13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>15</v>
@@ -747,24 +814,27 @@
         <v>16</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
+      <c r="K12" s="13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>15</v>
@@ -773,24 +843,27 @@
         <v>16</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
+      <c r="K13" s="13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>15</v>
@@ -799,24 +872,27 @@
         <v>16</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="5"/>
+      <c r="K14" s="13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>15</v>
@@ -825,24 +901,27 @@
         <v>16</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="5"/>
+      <c r="K15" s="13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>15</v>
@@ -851,33 +930,36 @@
         <v>16</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="5"/>
+      <c r="K16" s="13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="H17" s="13"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="12"/>
+        <v>44</v>
+      </c>
+      <c r="B18" s="14"/>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
@@ -892,10 +974,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="12" t="s">
         <v>45</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="C20" s="6"/>
     </row>
@@ -927,10 +1009,13 @@
       <c r="I21" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="J21" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>15</v>
@@ -939,29 +1024,113 @@
         <v>16</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>29</v>
+        <v>49</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
+      <c r="A23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="J23" s="13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-    </row>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" customFormat="false" ht="18.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="18.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="19.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -984,11 +1153,11 @@
   </sheetPr>
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.3984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
@@ -996,12 +1165,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1009,277 +1178,277 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>51</v>
+      <c r="A3" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12"/>
+      <c r="A4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
-        <v>55</v>
+      <c r="A7" s="14" t="s">
+        <v>68</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>51</v>
+        <v>65</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12"/>
-      <c r="C8" s="12"/>
+      <c r="A8" s="14"/>
+      <c r="C8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="12"/>
+        <v>69</v>
+      </c>
+      <c r="B9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="16"/>
+        <v>70</v>
+      </c>
+      <c r="C10" s="20"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="C11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>61</v>
+      <c r="A13" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>61</v>
+      <c r="A14" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="D15" s="12"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="12"/>
+        <v>76</v>
+      </c>
+      <c r="B16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17"/>
+        <v>77</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="18"/>
+      <c r="E18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="I19" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="J19" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="K19" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="L19" s="20" t="s">
-        <v>42</v>
+      <c r="J19" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="L19" s="24" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="35.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="12" t="s">
-        <v>70</v>
+      <c r="B20" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12" t="s">
-        <v>71</v>
+        <v>64</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="13"/>
-      <c r="H20" s="21" t="s">
-        <v>72</v>
+      <c r="G20" s="15"/>
+      <c r="H20" s="25" t="s">
+        <v>85</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L20" s="13" t="s">
-        <v>74</v>
+        <v>86</v>
+      </c>
+      <c r="L20" s="15" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="38.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="12" t="s">
-        <v>75</v>
+      <c r="B21" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>74</v>
+      <c r="G21" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>78</v>
+      <c r="A22" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="12"/>
-      <c r="I22" s="13" t="s">
-        <v>74</v>
+      <c r="G22" s="14"/>
+      <c r="I22" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="21"/>
-      <c r="J23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="25"/>
+      <c r="J23" s="15"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="22"/>
-      <c r="I24" s="13"/>
+      <c r="B24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="26"/>
+      <c r="I24" s="15"/>
     </row>
     <row r="25" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="21"/>
-      <c r="B25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="I25" s="13"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="I25" s="15"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="12"/>
+      <c r="B26" s="14"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="12"/>
+      <c r="B27" s="14"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="12"/>
+      <c r="B28" s="14"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="12"/>
+      <c r="B29" s="14"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="12"/>
+      <c r="B30" s="14"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="12"/>
+      <c r="B31" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
BIS-1002: Changed Import so Internal Property Assignment is not a separate column but '$$' prefix
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/systemtest/asapi/v3/test_files/import/import_internal_type.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/systemtest/asapi/v3/test_files/import/import_internal_type.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="96">
   <si>
     <t xml:space="preserve">DATASET_TYPE</t>
   </si>
@@ -101,7 +101,10 @@
     <t xml:space="preserve">IST</t>
   </si>
   <si>
-    <t xml:space="preserve">Internal Assignment</t>
+    <t xml:space="preserve">Pattern Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pattern</t>
   </si>
   <si>
     <t xml:space="preserve">SUPPLIER</t>
@@ -155,6 +158,18 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
+    <t xml:space="preserve">$FOR_WHAT_INTERNAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For what internal?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PATTERN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.*</t>
+  </si>
+  <si>
     <t xml:space="preserve">EXPERIMENT_TYPE</t>
   </si>
   <si>
@@ -176,10 +191,7 @@
     <t xml:space="preserve">Enter the code of the object type for which the collection is used</t>
   </si>
   <si>
-    <t xml:space="preserve">$FOR_WHAT_INTERNAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For what internal?</t>
+    <t xml:space="preserve">$$FOR_WHAT_INTERNAL</t>
   </si>
   <si>
     <t xml:space="preserve">VOCABULARY_TYPE</t>
@@ -309,7 +321,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -363,6 +375,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -373,28 +391,8 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -462,7 +460,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -511,11 +509,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -527,15 +521,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -543,11 +533,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -555,15 +545,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -588,13 +578,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.41796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.83"/>
@@ -770,8 +760,11 @@
       <c r="J10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="4" t="s">
         <v>26</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -799,13 +792,11 @@
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="13" t="s">
-        <v>15</v>
-      </c>
+      <c r="K11" s="12"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>15</v>
@@ -814,27 +805,25 @@
         <v>16</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="13" t="s">
-        <v>15</v>
-      </c>
+      <c r="K12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>15</v>
@@ -843,27 +832,25 @@
         <v>16</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="13" t="s">
-        <v>15</v>
-      </c>
+      <c r="K13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>15</v>
@@ -872,27 +859,25 @@
         <v>16</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="13" t="s">
-        <v>15</v>
-      </c>
+      <c r="K14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>15</v>
@@ -901,27 +886,25 @@
         <v>16</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="13" t="s">
-        <v>15</v>
-      </c>
+      <c r="K15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>15</v>
@@ -930,118 +913,119 @@
         <v>16</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="13" t="s">
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="14"/>
-    </row>
-    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="8"/>
+      <c r="K17" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="13"/>
+    </row>
+    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B20" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H22" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J21" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J22" s="13" t="s">
-        <v>15</v>
-      </c>
+      <c r="J22" s="15"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>51</v>
+      <c r="A23" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>15</v>
@@ -1049,89 +1033,110 @@
       <c r="C23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="5" t="s">
+      <c r="E24" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5" t="s">
+      <c r="G24" s="5"/>
+      <c r="H24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="8"/>
-      <c r="J23" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-    </row>
-    <row r="25" customFormat="false" ht="18.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="0"/>
-      <c r="C25" s="0"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="18.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="18.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="0"/>
-    </row>
-    <row r="27" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="C27" s="0"/>
     </row>
-    <row r="28" customFormat="false" ht="19.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="18" t="s">
+    <row r="28" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="19.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="18" t="s">
+      <c r="B29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="1" t="s">
+    <row r="30" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="0" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C30" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1157,7 +1162,7 @@
       <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.41796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
@@ -1165,12 +1170,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="14"/>
+        <v>67</v>
+      </c>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1178,277 +1183,277 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
-        <v>64</v>
+      <c r="A3" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14"/>
+      <c r="A4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="14"/>
+        <v>70</v>
+      </c>
+      <c r="B5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="A8" s="13"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="14"/>
+        <v>73</v>
+      </c>
+      <c r="B9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="20"/>
+        <v>74</v>
+      </c>
+      <c r="C10" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="14"/>
+        <v>50</v>
+      </c>
+      <c r="C11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>74</v>
+      <c r="A13" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>74</v>
+      <c r="A14" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="D15" s="14"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="D15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="14"/>
+        <v>80</v>
+      </c>
+      <c r="B16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21"/>
+        <v>81</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="22"/>
+      <c r="E18" s="20"/>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I19" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="I19" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J19" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="K19" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L19" s="24" t="s">
-        <v>43</v>
+      <c r="J19" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="35.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="14" t="s">
-        <v>83</v>
+      <c r="B20" s="13" t="s">
+        <v>87</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14" t="s">
-        <v>84</v>
+        <v>68</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13" t="s">
+        <v>88</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="25" t="s">
-        <v>85</v>
+      <c r="G20" s="14"/>
+      <c r="H20" s="23" t="s">
+        <v>89</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L20" s="15" t="s">
-        <v>87</v>
+        <v>90</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="38.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="14" t="s">
-        <v>88</v>
+      <c r="B21" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="G21" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I21" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="22" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>91</v>
+      <c r="A22" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>95</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="14"/>
-      <c r="I22" s="15" t="s">
-        <v>87</v>
+      <c r="G22" s="13"/>
+      <c r="I22" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="25"/>
-      <c r="J23" s="15"/>
+      <c r="B23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="23"/>
+      <c r="J23" s="14"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="26"/>
-      <c r="I24" s="15"/>
+      <c r="B24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="24"/>
+      <c r="I24" s="14"/>
     </row>
     <row r="25" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="25"/>
-      <c r="B25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="I25" s="15"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="I25" s="14"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="14"/>
+      <c r="B26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="14"/>
+      <c r="B27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="14"/>
+      <c r="B28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="14"/>
+      <c r="B29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="14"/>
+      <c r="B30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="14"/>
+      <c r="B31" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
BIS-1002: Fixed vocabulary terms import of internal vocabularies
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/systemtest/asapi/v3/test_files/import/import_internal_type.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/systemtest/asapi/v3/test_files/import/import_internal_type.xlsx
@@ -580,13 +580,13 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.41796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.16"/>
@@ -1159,10 +1159,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.41796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>

</xml_diff>